<commit_message>
김시우 UpgradeButton Passive 구현
김시우 UpgradeButton Passive 구현
</commit_message>
<xml_diff>
--- a/Design/DataTable/UpgradeButton.xlsx
+++ b/Design/DataTable/UpgradeButton.xlsx
@@ -21,40 +21,40 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <x:si>
+    <x:t>String</x:t>
+  </x:si>
+  <x:si>
+    <x:t>자원</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ID</x:t>
+  </x:si>
+  <x:si>
+    <x:t>int</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Resource</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Type</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Korean</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Passive</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tower</x:t>
+  </x:si>
+  <x:si>
     <x:t>Category_Num</x:t>
   </x:si>
   <x:si>
-    <x:t>Resource</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자원</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ID</x:t>
+    <x:t>타워</x:t>
   </x:si>
   <x:si>
     <x:t>패시브</x:t>
-  </x:si>
-  <x:si>
-    <x:t>int</x:t>
-  </x:si>
-  <x:si>
-    <x:t>타워</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Passive</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tower</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Korean</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Type</x:t>
-  </x:si>
-  <x:si>
-    <x:t>String</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -819,7 +819,7 @@
   <x:dimension ref="A1:D6"/>
   <x:sheetViews>
     <x:sheetView showGridLines="0" tabSelected="1" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="D3" activeCellId="0" sqref="D3:D3"/>
+      <x:selection activeCell="D5" activeCellId="0" sqref="D5:D5"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.550000000000001"/>
@@ -830,30 +830,30 @@
   <x:sheetData>
     <x:row r="1" spans="1:4" ht="16.399999999999999">
       <x:c r="A1" s="3" t="s">
-        <x:v>3</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="B1" s="3" t="s">
-        <x:v>10</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="C1" s="3" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D1" s="3" t="s">
         <x:v>9</x:v>
-      </x:c>
-      <x:c r="D1" s="3" t="s">
-        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4" ht="16.399999999999999">
       <x:c r="A2" s="3" t="s">
-        <x:v>5</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B2" s="3" t="s">
-        <x:v>11</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="C2" s="3" t="s">
-        <x:v>11</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="D2" s="3" t="s">
-        <x:v>5</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4" ht="16.399999999999999">
@@ -864,7 +864,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="C3" s="3" t="s">
-        <x:v>6</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D3" s="3">
         <x:v>13</x:v>
@@ -875,10 +875,10 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B4" s="3" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C4" s="3" t="s">
         <x:v>1</x:v>
-      </x:c>
-      <x:c r="C4" s="3" t="s">
-        <x:v>2</x:v>
       </x:c>
       <x:c r="D4" s="3">
         <x:v>4</x:v>
@@ -892,10 +892,10 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C5" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D5" s="3">
         <x:v>4</x:v>
-      </x:c>
-      <x:c r="D5" s="3">
-        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:1">

</xml_diff>